<commit_message>
Updated treatment of SAM coverage
</commit_message>
<xml_diff>
--- a/Projects/Tanzania/data/regional/InputForCode_Dodoma.xlsx
+++ b/Projects/Tanzania/data/regional/InputForCode_Dodoma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/Projects/Tanzania/data/regional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A8F32D78-B798-F640-945A-D97102A4DEAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{27A31847-8B3D-5244-AFF6-5F4446F04B29}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="27" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="47" r:id="rId1"/>
@@ -14985,6 +14985,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14995,11 +15000,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -15235,7 +15235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -25427,8 +25427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25978,7 +25978,7 @@
         <v>147</v>
       </c>
       <c r="B39" s="120">
-        <v>4.3999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="C39" s="145">
         <v>0.95</v>
@@ -25993,7 +25993,7 @@
         <v>148</v>
       </c>
       <c r="B40" s="120">
-        <v>0</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="C40" s="145">
         <v>0.95</v>

</xml_diff>